<commit_message>
Se actualizo el proyecto
</commit_message>
<xml_diff>
--- a/Proyecto/RDLC_titanic_clean.xlsx
+++ b/Proyecto/RDLC_titanic_clean.xlsx
@@ -2888,7 +2888,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daly, Mr. Peter Denis </t>
+          <t>Daly, Mr. Peter Denis</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -9794,7 +9794,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bryhl, Miss. Dagmar Jenny Ingeborg </t>
+          <t>Bryhl, Miss. Dagmar Jenny Ingeborg</t>
         </is>
       </c>
       <c r="E216" t="n">
@@ -10449,7 +10449,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t xml:space="preserve">Davies, Mrs. John Morgan (Elizabeth Agnes Mary White) </t>
+          <t>Davies, Mrs. John Morgan (Elizabeth Agnes Mary White)</t>
         </is>
       </c>
       <c r="E231" t="n">
@@ -11314,7 +11314,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hewlett, Mrs. (Mary D Kingcome) </t>
+          <t>Hewlett, Mrs. (Mary D Kingcome)</t>
         </is>
       </c>
       <c r="E251" t="n">

</xml_diff>